<commit_message>
(debug): fix export all
</commit_message>
<xml_diff>
--- a/student_timetable/1213_timetable.xlsx
+++ b/student_timetable/1213_timetable.xlsx
@@ -686,7 +686,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>8:00 to 9:00(L + T)</t>
+          <t>7:00 to 8:00(L + T)</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="D12" s="6" t="n">
-        <v>65432</v>
+        <v>234</v>
       </c>
       <c r="E12" s="6" t="n">
         <v/>

</xml_diff>